<commit_message>
changed LDO regulator to active one in stock
</commit_message>
<xml_diff>
--- a/pcb_boards/BOM.xlsx
+++ b/pcb_boards/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jelvani\Desktop\rurover\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\LAB PROJECTS\truck\rurover\pcb_boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7594CF81-C96C-44ED-AD4B-61D31691E5CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC47EDEA-51CB-46E2-A143-B6568D1BD032}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32280" yWindow="39030" windowWidth="29040" windowHeight="15840" xr2:uid="{52100737-4076-4ABF-A2A2-DD93ACAF2C6B}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{52100737-4076-4ABF-A2A2-DD93ACAF2C6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="77">
   <si>
     <t>Part</t>
   </si>
@@ -109,15 +109,6 @@
     <t>IC1</t>
   </si>
   <si>
-    <t>MC33269ST-5.0T3</t>
-  </si>
-  <si>
-    <t>MC33269ST-3.3T3</t>
-  </si>
-  <si>
-    <t>SOT223</t>
-  </si>
-  <si>
     <t>PWR_IN</t>
   </si>
   <si>
@@ -205,15 +196,6 @@
     <t>DPDT</t>
   </si>
   <si>
-    <t>TDK</t>
-  </si>
-  <si>
-    <t>C3216X5R1C476M160AB</t>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 1206 16VDC 47uF 20% X5R 1.6mm</t>
-  </si>
-  <si>
     <t>SMD/SMT</t>
   </si>
   <si>
@@ -229,9 +211,6 @@
     <t>SMA (DO-214AC)</t>
   </si>
   <si>
-    <t>47uF</t>
-  </si>
-  <si>
     <t>OSRAM Opto Semiconductors Inc.</t>
   </si>
   <si>
@@ -247,15 +226,6 @@
     <t>1206</t>
   </si>
   <si>
-    <t>ON Semiconductor</t>
-  </si>
-  <si>
-    <t>MC33275ST-5.0T3</t>
-  </si>
-  <si>
-    <t>Linear Voltage Regulator IC 1 Output 300mA SOT-223</t>
-  </si>
-  <si>
     <t>Panasonic</t>
   </si>
   <si>
@@ -269,6 +239,42 @@
   </si>
   <si>
     <t>1kOhms</t>
+  </si>
+  <si>
+    <t>LM2937IMP-5.0</t>
+  </si>
+  <si>
+    <t>SOT-223-4</t>
+  </si>
+  <si>
+    <t>LDO Voltage Regulators 500 MA LDO REG</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>LM2937IMP-5.0/NOPB</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>C1206X104K5RAC3316</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 50V 0.1uF X7R AUTO 5mm Flex VW 80808</t>
+  </si>
+  <si>
+    <t>C1206C106Z4VACTU</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 16V 10uF Y5V 1206 -20/80%</t>
   </si>
 </sst>
 </file>
@@ -697,22 +703,22 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.23046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.69140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.53515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.4609375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.3828125" customWidth="1"/>
-    <col min="7" max="7" width="15.61328125" customWidth="1"/>
-    <col min="8" max="8" width="16.69140625" customWidth="1"/>
+    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.375" customWidth="1"/>
+    <col min="7" max="7" width="15.625" customWidth="1"/>
+    <col min="8" max="8" width="16.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -735,62 +741,62 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -801,22 +807,22 @@
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -825,22 +831,22 @@
         <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -849,22 +855,22 @@
         <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -873,22 +879,22 @@
         <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -897,241 +903,241 @@
         <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A10" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>